<commit_message>
Rotated several components to fit manufacturer's placement
</commit_message>
<xml_diff>
--- a/cam/RP2040-Eins-20231007-JLCPCB-CPL-SOIC.xlsx
+++ b/cam/RP2040-Eins-20231007-JLCPCB-CPL-SOIC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\KiCad\7.0\projects\RP2040-Eins\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BC6548-27C5-4880-931C-EDAA264A5026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79E849E-5658-4873-98A2-33E6936E7329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13992" yWindow="2556" windowWidth="14040" windowHeight="14292" xr2:uid="{D2A07367-EB26-4D3C-95B3-13C76D9B899A}"/>
+    <workbookView xWindow="1080" yWindow="24" windowWidth="14040" windowHeight="14292" xr2:uid="{D2A07367-EB26-4D3C-95B3-13C76D9B899A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C0E679-E78B-48F3-874D-D3B284C2D2EB}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:XFD60"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1264,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="E38">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1281,7 +1281,7 @@
         <v>1</v>
       </c>
       <c r="E39">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1587,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="E57">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1621,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1638,7 +1638,7 @@
         <v>1</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>